<commit_message>
Consultar Produto Tela Principal
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/hub_tdd/testData/exceldoc.xlsx
+++ b/src/br/com/rsinet/hub_tdd/testData/exceldoc.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juliana.silva\Documents\workspace\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D5632DF-C073-4A01-B5A0-428A4712DC4C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3C1DF4E7-EA79-4F4B-AF1C-B5CFA2FFAEB5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{CA62D8A7-78DB-4A27-B65E-C7B0014626B4}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="20790" windowHeight="11820" xr2:uid="{CA62D8A7-78DB-4A27-B65E-C7B0014626B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>User Name</t>
   </si>
@@ -91,6 +87,9 @@
   </si>
   <si>
     <t>SP</t>
+  </si>
+  <si>
+    <t>Regiane</t>
   </si>
 </sst>
 </file>
@@ -471,7 +470,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +525,7 @@
     </row>
     <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Terminei o Screenshot, e comecei a fazer os log
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/hub_tdd/testData/exceldoc.xlsx
+++ b/src/br/com/rsinet/hub_tdd/testData/exceldoc.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9BEB1ADC-2313-45A1-B052-B526CA6DB3B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D69ADF69-EA32-402D-AD43-4D4D56CD1529}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="20490" windowHeight="13800" xr2:uid="{CA62D8A7-78DB-4A27-B65E-C7B0014626B4}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20520" windowHeight="11820" xr2:uid="{CA62D8A7-78DB-4A27-B65E-C7B0014626B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>User Name</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Postal Code</t>
   </si>
   <si>
-    <t xml:space="preserve">Juliana </t>
-  </si>
-  <si>
     <t>1415Ju</t>
   </si>
   <si>
@@ -83,7 +80,7 @@
     <t>SP</t>
   </si>
   <si>
-    <t>Brunoooooa</t>
+    <t>Julianaju</t>
   </si>
 </sst>
 </file>
@@ -473,7 +470,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,37 +525,37 @@
     </row>
     <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
       </c>
       <c r="G2">
         <v>11987654321</v>
       </c>
       <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
       </c>
       <c r="L2">
         <v>123456</v>

</xml_diff>

<commit_message>
Refatorei o codigo, termineti os log
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/hub_tdd/testData/exceldoc.xlsx
+++ b/src/br/com/rsinet/hub_tdd/testData/exceldoc.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D69ADF69-EA32-402D-AD43-4D4D56CD1529}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juliana.silva\Desktop\workspace-nova\ProjetoTDDJuliana\src\br\com\rsinet\hub_tdd\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F646CFC2-0D20-4BC6-89D1-EAA71DFC15C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20520" windowHeight="11820" xr2:uid="{CA62D8A7-78DB-4A27-B65E-C7B0014626B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CA62D8A7-78DB-4A27-B65E-C7B0014626B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -470,7 +474,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>